<commit_message>
Import notes when we have them
</commit_message>
<xml_diff>
--- a/public/import_template.xlsx
+++ b/public/import_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\rover\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rover\Code\bmac\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2096888C-D0C5-48BC-849C-0288534E97A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B467B0F9-B540-467B-9780-1EB5122FCFBD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1905" yWindow="1905" windowWidth="21600" windowHeight="11385" xr2:uid="{D04AF5E1-FD0B-423F-91F9-BDC72DF41FA8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D04AF5E1-FD0B-423F-91F9-BDC72DF41FA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Call Sign</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>Route</t>
+  </si>
+  <si>
+    <t>Notes</t>
   </si>
 </sst>
 </file>
@@ -421,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91403348-4099-4258-BDAA-3E7E76500E16}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -436,7 +439,7 @@
     <col min="7" max="7" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -457,6 +460,9 @@
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Flight Notes for all event types (#112)
* Import notes when we have them

* Show notes when we have them

* Move Cancel Booking button outside form

This was the reason why that button was below the edit button 🤦‍♂️

* Notes can now also be added/updated when creating/updating a booking
</commit_message>
<xml_diff>
--- a/public/import_template.xlsx
+++ b/public/import_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\rover\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rover\Code\bmac\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2096888C-D0C5-48BC-849C-0288534E97A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B467B0F9-B540-467B-9780-1EB5122FCFBD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1905" yWindow="1905" windowWidth="21600" windowHeight="11385" xr2:uid="{D04AF5E1-FD0B-423F-91F9-BDC72DF41FA8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D04AF5E1-FD0B-423F-91F9-BDC72DF41FA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Call Sign</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>Route</t>
+  </si>
+  <si>
+    <t>Notes</t>
   </si>
 </sst>
 </file>
@@ -421,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91403348-4099-4258-BDAA-3E7E76500E16}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -436,7 +439,7 @@
     <col min="7" max="7" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -457,6 +460,9 @@
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Making sure import uses correct values. Fix #316
</commit_message>
<xml_diff>
--- a/public/import_template.xlsx
+++ b/public/import_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rover\Code\bmac\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveroverts/code/sites/bmac/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B467B0F9-B540-467B-9780-1EB5122FCFBD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{350A604C-C307-1B42-970D-B497DA28A4A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D04AF5E1-FD0B-423F-91F9-BDC72DF41FA8}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="15840" xr2:uid="{D04AF5E1-FD0B-423F-91F9-BDC72DF41FA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -44,9 +44,6 @@
     <t>Destination</t>
   </si>
   <si>
-    <t>EOBT</t>
-  </si>
-  <si>
     <t>ETA</t>
   </si>
   <si>
@@ -57,6 +54,9 @@
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>CTOT</t>
   </si>
 </sst>
 </file>
@@ -427,19 +427,19 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -450,19 +450,19 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>